<commit_message>
Fixed issue when no file saved
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>title</t>
   </si>
@@ -43,9 +43,15 @@
     <t>abstract</t>
   </si>
   <si>
+    <t>BERT: Pre-training of Deep Bidirectional Transformers for Language Understanding</t>
+  </si>
+  <si>
     <t>OCR-free Document Understanding Transformer</t>
   </si>
   <si>
+    <t>BART: Denoising Sequence-to-Sequence Pre-training for Natural Language Generation, Translation, and Comprehension</t>
+  </si>
+  <si>
     <t>Attention Is All You Need</t>
   </si>
   <si>
@@ -58,6 +64,27 @@
     <t>LayoutLMv2: Multi-modal Pre-training for Visually-Rich Document Understanding</t>
   </si>
   <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>Devlin, Jacob and Chang, Ming-Wei and Lee, Kenton and Toutanova, Kristina</t>
+  </si>
+  <si>
+    <t>arXiv</t>
+  </si>
+  <si>
+    <t>Devlin et al. - 2019 - BERT Pre-training of Deep Bidirectional Transform.pdf</t>
+  </si>
+  <si>
+    <t>Computer Science - Computation and Language</t>
+  </si>
+  <si>
+    <t>We introduce a new language representation model called BERT, which stands for Bidirectional Encoder Representations from Transformers. Unlike recent language representation models, BERT is designed to pre-train deep bidirectional representations from unlabeled text by jointly conditioning on both left and right context in all layers. As a result, the pre-trained BERT model can be fine-tuned with just one additional output layer to create state-of-the-art models for a wide range of tasks, such as question answering and language inference, without substantial task-specific architecture modifications. BERT is conceptually simple and empirically powerful. It obtains new state-of-the-art results on eleven natural language processing tasks, including pushing the GLUE score to 80.5% (7.7% point absolute improvement), MultiNLI accuracy to 86.7% (4.6% absolute improvement), SQuAD v1.1 question answering Test F1 to 93.2 (1.5 point absolute improvement) and SQuAD v2.0 Test F1 to 83.1 (5.1 point absolute improvement).</t>
+  </si>
+  <si>
     <t>October</t>
   </si>
   <si>
@@ -67,9 +94,6 @@
     <t>Kim, Geewook and Hong, Teakgyu and Yim, Moonbin and Nam, Jeongyeon and Park, Jinyoung and Yim, Jinyeong and Hwang, Wonseok and Yun, Sangdoo and Han, Dongyoon and Park, Seunghyun</t>
   </si>
   <si>
-    <t>arXiv</t>
-  </si>
-  <si>
     <t>Kim et al. - 2022 - OCR-free Document Understanding Transformer.pdf</t>
   </si>
   <si>
@@ -82,6 +106,18 @@
     <t>Understanding document images (e.g., invoices) is a core but challenging task since it requires complex functions such as reading text and a holistic understanding of the document. Current Visual Document Understanding (VDU) methods outsource the task of reading text to offthe-shelf Optical Character Recognition (OCR) engines and focus on the understanding task with the OCR outputs. Although such OCR-based approaches have shown promising performance, they suffer from 1) high computational costs for using OCR; 2) inflexibility of OCR models on languages or types of documents; 3) OCR error propagation to the subsequent process. To address these issues, in this paper, we introduce a novel OCR-free VDU model named Donut, which stands for Document understanding transformer. As the first step in OCR-free VDU research, we propose a simple architecture (i.e., Transformer) with a pre-training objective (i.e., cross-entropy loss). Donut is conceptually simple yet effective. Through extensive experiments and analyses, we show a simple OCR-free VDU model, Donut, achieves state-of-the-art performances on various VDU tasks in terms of both speed and accuracy. In addition, we offer a synthetic data generator that helps the model pre-training to be flexible in various languages and domains. The code, trained model, and synthetic data are available at https://github.com/clovaai/donut.</t>
   </si>
   <si>
+    <t>Lewis, Mike and Liu, Yinhan and Goyal, Naman and Ghazvininejad, Marjan and Mohamed, Abdelrahman and Levy, Omer and Stoyanov, Ves and Zettlemoyer, Luke</t>
+  </si>
+  <si>
+    <t>Lewis et al. - 2019 - BART Denoising Sequence-to-Sequence Pre-training .pdf</t>
+  </si>
+  <si>
+    <t>Computer Science - Computation and Language,Computer Science - Machine Learning,Statistics - Machine Learning</t>
+  </si>
+  <si>
+    <t>We present BART, a denoising autoencoder for pretraining sequence-to-sequence models. BART is trained by (1) corrupting text with an arbitrary noising function, and (2) learning a model to reconstruct the original text. It uses a standard Tranformer-based neural machine translation architecture which, despite its simplicity, can be seen as generalizing BERT (due to the bidirectional encoder), GPT (with the left-to-right decoder), and many other more recent pretraining schemes. We evaluate a number of noising approaches, finding the best performance by both randomly shuffling the order of the original sentences and using a novel in-filling scheme, where spans of text are replaced with a single mask token. BART is particularly effective when fine tuned for text generation but also works well for comprehension tasks. It matches the performance of RoBERTa with comparable training resources on GLUE and SQuAD, achieves new state-of-the-art results on a range of abstractive dialogue, question answering, and summarization tasks, with gains of up to 6 ROUGE. BART also provides a 1.1 BLEU increase over a back-translation system for machine translation, with only target language pretraining. We also report ablation experiments that replicate other pretraining schemes within the BART framework, to better measure which factors most influence end-task performance.</t>
+  </si>
+  <si>
     <t>2017</t>
   </si>
   <si>
@@ -134,9 +170,6 @@
   </si>
   <si>
     <t>Xu et al. - 2022 - LayoutLMv2 Multi-modal Pre-training for Visually-.pdf</t>
-  </si>
-  <si>
-    <t>Computer Science - Computation and Language</t>
   </si>
   <si>
     <t>Pre-training of text and layout has proved effective in a variety of visually-rich document understanding tasks due to its effective model architecture and the advantage of large-scale unlabeled scanned/digital-born documents. We propose LayoutLMv2 architecture with new pre-training tasks to model the interaction among text, layout, and image in a single multi-modal framework. Specifically, with a two-stream multi-modal Transformer encoder, LayoutLMv2 uses not only the existing masked visual-language modeling task but also the new text-image alignment and text-image matching tasks, which make it better capture the cross-modality interaction in the pre-training stage. Meanwhile, it also integrates a spatial-aware self-attention mechanism into the Transformer architecture so that the model can fully understand the relative positional relationship among different text blocks. Experiment results show that LayoutLMv2 outperforms LayoutLM by a large margin and achieves new state-ofthe-art results on a wide variety of downstream visually-rich document understanding tasks, including FUNSD (0.7895 \textrightarrow 0.8420), CORD (0.9493 \textrightarrow 0.9601), SROIE (0.9524 \textrightarrow 0.9781), Kleister-NDA (0.8340 \textrightarrow 0.8520), RVL-CDIP (0.9443 \textrightarrow 0.9564), and DocVQA (0.7295 \textrightarrow 0.8672). We made our model and code publicly available at https://aka.ms /layoutlmv2.</t>
@@ -508,13 +541,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="96" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" customWidth="1"/>
@@ -559,53 +592,55 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="96" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="H3" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="96" customHeight="1">
@@ -613,53 +648,51 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="96" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="I5" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="96" customHeight="1">
@@ -667,26 +700,80 @@
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="96" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="96" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tables (getter only local)
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>title</t>
   </si>
@@ -43,6 +43,9 @@
     <t>abstract</t>
   </si>
   <si>
+    <t>DocFormer: End-to-End Transformer for Document Understanding</t>
+  </si>
+  <si>
     <t>BERT: Pre-training of Deep Bidirectional Transformers for Language Understanding</t>
   </si>
   <si>
@@ -64,6 +67,27 @@
     <t>LayoutLMv2: Multi-modal Pre-training for Visually-Rich Document Understanding</t>
   </si>
   <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>Appalaraju, Srikar and Jasani, Bhavan and Kota, Bhargava Urala and Xie, Yusheng and Manmatha, R.</t>
+  </si>
+  <si>
+    <t>arXiv</t>
+  </si>
+  <si>
+    <t>Appalaraju et al. - 2021 - DocFormer End-to-End Transformer for Document Und.pdf</t>
+  </si>
+  <si>
+    <t>Computer Science - Computer Vision and Pattern Recognition</t>
+  </si>
+  <si>
+    <t>We present DocFormer -- a multi-modal transformer based architecture for the task of Visual Document Understanding (VDU). VDU is a challenging problem which aims to understand documents in their varied formats (forms, receipts etc.) and layouts. In addition, DocFormer is pre-trained in an unsupervised fashion using carefully designed tasks which encourage multi-modal interaction. DocFormer uses text, vision and spatial features and combines them using a novel multi-modal self-attention layer. DocFormer also shares learned spatial embeddings across modalities which makes it easy for the model to correlate text to visual tokens and vice versa. DocFormer is evaluated on 4 different datasets each with strong baselines. DocFormer achieves state-of-the-art results on all of them, sometimes beating models 4x its size (in no. of parameters).</t>
+  </si>
+  <si>
     <t>May</t>
   </si>
   <si>
@@ -73,9 +97,6 @@
     <t>Devlin, Jacob and Chang, Ming-Wei and Lee, Kenton and Toutanova, Kristina</t>
   </si>
   <si>
-    <t>arXiv</t>
-  </si>
-  <si>
     <t>Devlin et al. - 2019 - BERT Pre-training of Deep Bidirectional Transform.pdf</t>
   </si>
   <si>
@@ -155,9 +176,6 @@
   </si>
   <si>
     <t>Tschannen et al. - 2022 - Image-and-Language Understanding from Pixels Only.pdf</t>
-  </si>
-  <si>
-    <t>Computer Science - Computer Vision and Pattern Recognition</t>
   </si>
   <si>
     <t>Multimodal models are becoming increasingly effective, in part due to unified components, such as the Transformer architecture. However, multimodal models still often consist of many task- and modality-specific pieces and training procedures. For example, CLIP (Radford et al., 2021) trains independent text and image towers via a contrastive loss. We explore an additional unification: the use of a pure pixel-based model to perform image, text, and multimodal tasks. Our model is trained with contrastive loss alone, so we call it CLIP-Pixels Only (CLIPPO). CLIPPO uses a single encoder that processes both regular images and text rendered as images. CLIPPO performs image-based tasks such as retrieval and zero-shot image classification almost as well as CLIP, with half the number of parameters and no text-specific tower or embedding. When trained jointly via image-text contrastive learning and next-sentence contrastive learning, CLIPPO can perform well on natural language understanding tasks, without any word-level loss (language modelling or masked language modelling), outperforming pixel-based prior work. Surprisingly, CLIPPO can obtain good accuracy in visual question answering, simply by rendering the question and image together. Finally, we exploit the fact that CLIPPO does not require a tokenizer to show that it can achieve strong performance on multilingual multimodal retrieval without</t>
@@ -541,18 +559,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="96" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
     <col min="7" max="7" width="38.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" customWidth="1"/>
     <col min="9" max="9" width="192.7109375" customWidth="1"/>
@@ -592,26 +610,26 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="96" customHeight="1">
@@ -619,26 +637,24 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
         <v>29</v>
       </c>
@@ -648,78 +664,80 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="I4" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="96" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="G5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="96" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="I6" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="96" customHeight="1">
@@ -727,26 +745,26 @@
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="96" customHeight="1">
@@ -754,26 +772,53 @@
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="96" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New columns in xlsx can be added manually
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>title</t>
   </si>
@@ -25,6 +25,9 @@
     <t>year</t>
   </si>
   <si>
+    <t>category</t>
+  </si>
+  <si>
     <t>author</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t>2021</t>
   </si>
   <si>
+    <t>VDU</t>
+  </si>
+  <si>
     <t>Appalaraju, Srikar and Jasani, Bhavan and Kota, Bhargava Urala and Xie, Yusheng and Manmatha, R.</t>
   </si>
   <si>
@@ -85,6 +91,9 @@
     <t>Computer Science - Computer Vision and Pattern Recognition</t>
   </si>
   <si>
+    <t>Good image for comparison of VDU methods on page 2</t>
+  </si>
+  <si>
     <t>We present DocFormer -- a multi-modal transformer based architecture for the task of Visual Document Understanding (VDU). VDU is a challenging problem which aims to understand documents in their varied formats (forms, receipts etc.) and layouts. In addition, DocFormer is pre-trained in an unsupervised fashion using carefully designed tasks which encourage multi-modal interaction. DocFormer uses text, vision and spatial features and combines them using a novel multi-modal self-attention layer. DocFormer also shares learned spatial embeddings across modalities which makes it easy for the model to correlate text to visual tokens and vice versa. DocFormer is evaluated on 4 different datasets each with strong baselines. DocFormer achieves state-of-the-art results on all of them, sometimes beating models 4x its size (in no. of parameters).</t>
   </si>
   <si>
@@ -92,6 +101,9 @@
   </si>
   <si>
     <t>2019</t>
+  </si>
+  <si>
+    <t>Transformer Language Model</t>
   </si>
   <si>
     <t>Devlin, Jacob and Chang, Ming-Wei and Lee, Kenton and Toutanova, Kristina</t>
@@ -559,7 +571,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -568,15 +580,16 @@
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
-    <col min="7" max="7" width="38.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="192.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="38.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="10" max="10" width="192.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="96" customHeight="1">
+    <row r="1" spans="1:10" ht="96" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,221 +617,250 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="96" customHeight="1">
+    <row r="2" spans="1:10" ht="96" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="96" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="96" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
+      <c r="G4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="96" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="3" t="s">
+    <row r="5" spans="1:10" ht="96" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="96" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="96" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="96" customHeight="1">
+    <row r="6" spans="1:10" ht="96" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="96" customHeight="1">
+    <row r="7" spans="1:10" ht="96" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="96" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3" t="s">
-        <v>51</v>
+      <c r="E8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="96" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="3" t="s">
+    <row r="9" spans="1:10" ht="96" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="96" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>